<commit_message>
Update OUCD - complete version
</commit_message>
<xml_diff>
--- a/Sonstiges/Unity3D Assets Coasts.xlsx
+++ b/Sonstiges/Unity3D Assets Coasts.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\GitHub\NoRPG-docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15150"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$B$2:$I$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$B$2:$I$27</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="35">
   <si>
     <t>https://www.assetstore.unity3d.com/en/#!/content/19826</t>
   </si>
@@ -126,12 +121,18 @@
   </si>
   <si>
     <t>https://www.assetstore.unity3d.com/en/#!/content/45786</t>
+  </si>
+  <si>
+    <t>https://www.assetstore.unity3d.com/en/#!/content/52666</t>
+  </si>
+  <si>
+    <t>https://www.assetstore.unity3d.com/en/#!/content/71525</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0"/>
   </numFmts>
@@ -180,7 +181,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -323,12 +324,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -355,9 +365,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -662,7 +673,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -670,23 +681,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I26"/>
+  <dimension ref="B1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="55" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" customWidth="1"/>
-    <col min="10" max="11" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1076,8 +1087,8 @@
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
-        <v>1</v>
+      <c r="B23" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>30</v>
@@ -1085,68 +1096,113 @@
       <c r="D23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="E23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="I23" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="15">
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="15">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="5" t="s">
+    <row r="27" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I25" s="8">
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27" s="8">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12" t="s">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="I26" s="13">
-        <f>SUM(I3:I25)</f>
-        <v>240</v>
+      <c r="I28" s="13">
+        <f>SUM(I3:I27)</f>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:I24">
+  <autoFilter ref="B2:I26">
     <sortState ref="B3:I25">
       <sortCondition ref="I2:I24"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="I3:I23 I25">
+  <conditionalFormatting sqref="I3:I25 I27">
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
@@ -1160,7 +1216,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I25">
+  <conditionalFormatting sqref="I3:I27">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -1177,7 +1233,7 @@
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
     <hyperlink ref="B21" r:id="rId2" location="!/content/19826"/>
-    <hyperlink ref="B23" r:id="rId3" location="!/content/63165"/>
+    <hyperlink ref="B24" r:id="rId3" location="!/content/63165"/>
     <hyperlink ref="B11" r:id="rId4" location="!/content/65939"/>
     <hyperlink ref="B5" r:id="rId5" location="!/content/67201"/>
     <hyperlink ref="B9" r:id="rId6" location="!/content/72522"/>
@@ -1193,14 +1249,16 @@
     <hyperlink ref="B18" r:id="rId16" location="!/content/56822"/>
     <hyperlink ref="B15" r:id="rId17" location="!/content/58300"/>
     <hyperlink ref="B17" r:id="rId18" location="!/content/19973"/>
-    <hyperlink ref="B25" r:id="rId19" location="!/content/9312"/>
+    <hyperlink ref="B27" r:id="rId19" location="!/content/9312"/>
     <hyperlink ref="B22" r:id="rId20" location="!/content/49171"/>
     <hyperlink ref="B14" r:id="rId21" location="!/content/20054"/>
     <hyperlink ref="B10" r:id="rId22" location="!/content/66322"/>
-    <hyperlink ref="B24" r:id="rId23" location="!/content/45786"/>
+    <hyperlink ref="B26" r:id="rId23" location="!/content/45786"/>
+    <hyperlink ref="B23" r:id="rId24" location="!/content/52666"/>
+    <hyperlink ref="B25" r:id="rId25" location="!/content/71525"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -1213,7 +1271,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I3:I23 I25</xm:sqref>
+          <xm:sqref>I3:I25 I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{27FBA6FE-B4A8-4CB9-8964-F11684496BA6}">
@@ -1224,7 +1282,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I3:I25</xm:sqref>
+          <xm:sqref>I3:I27</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>